<commit_message>
experimentation for the dockerization of datacatalogue
</commit_message>
<xml_diff>
--- a/src/main/resources/data/variables/dementia_Plovdiv_v1.xlsx
+++ b/src/main/resources/data/variables/dementia_Plovdiv_v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="117">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">The age of the patient in years</t>
   </si>
   <si>
-    <t xml:space="preserve">{stays the same},  {corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}}</t>
+    <t xml:space="preserve">[stays the same],  [corresponds to one of the groups: {“-50y”},{”50-59y”},{”60-69y”},{”70-79y”},{”+80y”}]</t>
   </si>
   <si>
     <t xml:space="preserve">subjectageyears, agegroup</t>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t xml:space="preserve">Describes the tendency of the patient to use either the right or the left hand more naturally than the other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/root/demographics/Handedness</t>
   </si>
   <si>
     <t xml:space="preserve">Smoking</t>
@@ -512,22 +515,22 @@
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D2" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J28" activeCellId="0" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="67.914979757085"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="68.9838056680162"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.919028340081"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1011,23 +1014,25 @@
       <c r="H28" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,13 +1040,13 @@
         <v>13</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,13 +1054,13 @@
         <v>13</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,16 +1068,16 @@
         <v>13</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>